<commit_message>
missing value ignore and dynamic selectoption value
</commit_message>
<xml_diff>
--- a/atique.xlsx
+++ b/atique.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ur_sensei\Desktop\translation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424812FE-38FC-441E-8982-9C635C7D996F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D720B45-7D96-44E4-B787-A674F1C4E360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{98118860-C578-4587-916B-A7E3CA3C03BF}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2439" uniqueCount="1915">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2440" uniqueCount="1914">
   <si>
     <t>#</t>
   </si>
@@ -9931,15 +9931,12 @@
   <si>
     <t>பின்னர்  முன்னோக்கி என்ற பட்டனை Click செய்யவும்</t>
   </si>
-  <si>
-    <t>multicheck</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="75">
+  <fonts count="76">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -10408,6 +10405,12 @@
       <name val="Ui-Sans-Serif"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -10661,7 +10664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -11178,6 +11181,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14653,8 +14659,8 @@
   <dimension ref="A1:P91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K59" sqref="K59"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1"/>
@@ -16038,8 +16044,8 @@
       <c r="H59" s="65" t="s">
         <v>1004</v>
       </c>
-      <c r="I59" s="121" t="s">
-        <v>1914</v>
+      <c r="I59" s="198" t="s">
+        <v>1005</v>
       </c>
       <c r="J59" s="121" t="s">
         <v>1006</v>
@@ -16141,7 +16147,7 @@
         <v>1010</v>
       </c>
       <c r="I63" s="121" t="s">
-        <v>1011</v>
+        <v>828</v>
       </c>
       <c r="J63" s="121"/>
       <c r="K63" s="65" t="s">
@@ -16477,7 +16483,9 @@
       <c r="F78" s="165"/>
       <c r="G78" s="121"/>
       <c r="H78" s="121"/>
-      <c r="I78" s="121"/>
+      <c r="I78" s="121" t="s">
+        <v>828</v>
+      </c>
       <c r="J78" s="121"/>
       <c r="K78" s="162" t="s">
         <v>1058</v>
@@ -16868,6 +16876,7 @@
     <mergeCell ref="A63:A84"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -23034,6 +23043,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="bdbedefb-8a5a-49d5-aad5-33b2c71b0a4d" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00591925-1995-4bf8-8d28-1f7cbeda4924">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A595C2436754DD4192B3BEE0FFE1ED0A" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="93ba19257e65125414350f132367e985">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="00591925-1995-4bf8-8d28-1f7cbeda4924" xmlns:ns3="bdbedefb-8a5a-49d5-aad5-33b2c71b0a4d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b2a6491f746e84da8ae5f2642b9bcf21" ns2:_="" ns3:_="">
     <xsd:import namespace="00591925-1995-4bf8-8d28-1f7cbeda4924"/>
@@ -23262,27 +23291,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="bdbedefb-8a5a-49d5-aad5-33b2c71b0a4d" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00591925-1995-4bf8-8d28-1f7cbeda4924">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{319AAEED-380C-474B-BD5E-BD614C666CFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bdbedefb-8a5a-49d5-aad5-33b2c71b0a4d"/>
+    <ds:schemaRef ds:uri="00591925-1995-4bf8-8d28-1f7cbeda4924"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32FAF7A7-D9AD-4A85-9EE8-33F1ACC4911B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72B4B015-2F19-4BB0-A14D-E91581C50494}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23299,23 +23327,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{319AAEED-380C-474B-BD5E-BD614C666CFF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bdbedefb-8a5a-49d5-aad5-33b2c71b0a4d"/>
-    <ds:schemaRef ds:uri="00591925-1995-4bf8-8d28-1f7cbeda4924"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{32FAF7A7-D9AD-4A85-9EE8-33F1ACC4911B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>